<commit_message>
speed up loadcases generators by disabling UI
</commit_message>
<xml_diff>
--- a/m100_Tools_And_Helpers/DataFiles/11 Loadcases.xlsx
+++ b/m100_Tools_And_Helpers/DataFiles/11 Loadcases.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rob\repos\LusasNoteBooks\m100_Tools_And_Helpers\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rob\repos\LusasNoteBooks\m100_Tools_And_Helpers\DataFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{428C9DD3-1805-49D4-BF34-E5A9EC6EFC10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1ACEA71-22E9-42C0-944A-36561C919645}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="64">
   <si>
     <t>Self Weight</t>
   </si>
@@ -60,9 +60,6 @@
     <t>Shrinkage</t>
   </si>
   <si>
-    <t>Temperature</t>
-  </si>
-  <si>
     <t>Analysis</t>
   </si>
   <si>
@@ -117,33 +114,12 @@
     <t>Traffic 10</t>
   </si>
   <si>
-    <t>Name = Name of envelope to be created</t>
-  </si>
-  <si>
-    <t>Loadcases = Name of loadcases to be included in the envelope</t>
-  </si>
-  <si>
-    <t>FindSimilar = Use all loadsets that start with the loadcase name</t>
-  </si>
-  <si>
-    <t>Name = Name of loadcase to be created</t>
-  </si>
-  <si>
-    <t>Count = Number of similar loadcases to be created = default empty = 1</t>
-  </si>
-  <si>
-    <t>Analysis = Name of the analysis in which to create the loadcase</t>
-  </si>
-  <si>
     <t>Prestress</t>
   </si>
   <si>
     <t>Gravity</t>
   </si>
   <si>
-    <t>Gravity = Automatically apply gravity to the loadcase</t>
-  </si>
-  <si>
     <t>Settlement Envelope</t>
   </si>
   <si>
@@ -153,9 +129,6 @@
     <t>TLO Traffic Envelope</t>
   </si>
   <si>
-    <t>Thermal Envelope</t>
-  </si>
-  <si>
     <t>Rail Load Characteristic</t>
   </si>
   <si>
@@ -180,9 +153,6 @@
     <t>Folder</t>
   </si>
   <si>
-    <t>Folder = Folder for grouping envelopes in tree view</t>
-  </si>
-  <si>
     <t>Explosion</t>
   </si>
   <si>
@@ -214,6 +184,51 @@
   </si>
   <si>
     <t>03 Seismic Actions</t>
+  </si>
+  <si>
+    <t>Thermal Uniform Pos</t>
+  </si>
+  <si>
+    <t>Thermal Uniform Neg</t>
+  </si>
+  <si>
+    <t>Thermal Gradient Pos</t>
+  </si>
+  <si>
+    <t>Thermal Gradient Neg</t>
+  </si>
+  <si>
+    <t>Thermal Uniform</t>
+  </si>
+  <si>
+    <t>Thermal Gradient</t>
+  </si>
+  <si>
+    <t>Breaking and Traction</t>
+  </si>
+  <si>
+    <t>Braking</t>
+  </si>
+  <si>
+    <t>Traction</t>
+  </si>
+  <si>
+    <t>Horizontal Envelope</t>
+  </si>
+  <si>
+    <t>Horizontal</t>
+  </si>
+  <si>
+    <t>Breaking</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Traction </t>
+  </si>
+  <si>
+    <t>Earth pressure vertical</t>
+  </si>
+  <si>
+    <t>Earth pressure horizontal</t>
   </si>
 </sst>
 </file>
@@ -294,6 +309,290 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>7620</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>102870</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8D482309-D676-41D2-912F-8CFF6D929BF6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5730240" y="190500"/>
+          <a:ext cx="4467225" cy="1009650"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="1" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Name = Name of loadcase to be created</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="1" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Count = Number of similar loadcases to be created = default empty = 1</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" b="1">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="1" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Gravity = Automatically apply gravity to the loadcase</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" b="1">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="1" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Analysis = Name of the analysis in which to create the loadcase</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" b="1">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+          <a:endParaRPr lang="en-GB" sz="1100" b="1">
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>22860</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>15240</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>588645</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>112395</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4FD91395-8B3E-4250-A32D-BCA9EB6DD3F1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6347460" y="198120"/>
+          <a:ext cx="3613785" cy="828675"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="1" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Name = Name of envelope to be created</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="1" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Loadcases = Name of loadcases to be included in the envelope</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="1" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>FindSimilar = Use all loadsets that start with the loadcase name</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="1" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Folder = Folder for grouping envelopes in treeview</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-GB" sz="1100" b="1">
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -559,15 +858,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I16"/>
+  <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.88671875" customWidth="1"/>
     <col min="2" max="3" width="8.88671875" style="3"/>
     <col min="4" max="4" width="25.109375" bestFit="1" customWidth="1"/>
   </cols>
@@ -580,10 +879,10 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
@@ -591,27 +890,21 @@
         <v>0</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>29</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="I2" s="2"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="I3" s="2" t="s">
-        <v>30</v>
-      </c>
+      <c r="I3" s="2"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>5</v>
       </c>
-      <c r="I4" s="2" t="s">
-        <v>34</v>
-      </c>
+      <c r="I4" s="2"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
@@ -620,9 +913,7 @@
       <c r="B5" s="3">
         <v>4</v>
       </c>
-      <c r="I5" s="2" t="s">
-        <v>31</v>
-      </c>
+      <c r="I5" s="2"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
@@ -631,72 +922,48 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="3">
-        <v>2</v>
+        <v>63</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" s="3">
-        <v>10</v>
-      </c>
-      <c r="D8" t="s">
-        <v>12</v>
+        <v>62</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" s="3">
-        <v>4</v>
+        <v>49</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>11</v>
+        <v>50</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>32</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D11" t="s">
-        <v>32</v>
+        <v>51</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>41</v>
-      </c>
-      <c r="B12" s="3">
-        <v>5</v>
-      </c>
-      <c r="D12" t="s">
-        <v>39</v>
+        <v>52</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>42</v>
+        <v>8</v>
       </c>
       <c r="B13" s="3">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D13" t="s">
-        <v>39</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>48</v>
+        <v>60</v>
       </c>
       <c r="B14" s="3">
         <v>2</v>
@@ -704,7 +971,7 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>49</v>
+        <v>61</v>
       </c>
       <c r="B15" s="3">
         <v>2</v>
@@ -712,28 +979,99 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="B16" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>9</v>
+      </c>
+      <c r="B17" s="3">
         <v>4</v>
       </c>
-      <c r="D16" t="s">
-        <v>53</v>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>25</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D19" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>32</v>
+      </c>
+      <c r="B20" s="3">
+        <v>5</v>
+      </c>
+      <c r="D20" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>33</v>
+      </c>
+      <c r="B21" s="3">
+        <v>5</v>
+      </c>
+      <c r="D21" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>38</v>
+      </c>
+      <c r="B22" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>39</v>
+      </c>
+      <c r="B23" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>42</v>
+      </c>
+      <c r="B24" s="3">
+        <v>4</v>
+      </c>
+      <c r="D24" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{803832CE-E52E-47CE-865F-4A6C7DB9A262}">
-  <dimension ref="A1:G20"/>
+  <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -749,266 +1087,315 @@
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D2" t="s">
-        <v>55</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>26</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="G2" s="2"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D3" t="s">
-        <v>56</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>27</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="G3" s="2"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>38</v>
+        <v>53</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>53</v>
       </c>
       <c r="C4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D4" t="s">
-        <v>56</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>28</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="G4" s="2"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>37</v>
+        <v>54</v>
       </c>
       <c r="B5" t="s">
-        <v>16</v>
+        <v>54</v>
+      </c>
+      <c r="C5" t="s">
+        <v>13</v>
       </c>
       <c r="D5" t="s">
-        <v>56</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>47</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="G5" s="2"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="B6" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D6" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="B7" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D7" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="B8" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D8" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="B9" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D9" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="B10" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D10" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="B11" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D11" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="B12" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D12" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="B13" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D13" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="B14" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D14" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="B15" t="s">
-        <v>41</v>
-      </c>
-      <c r="C15" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="D15" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="B16" t="s">
-        <v>42</v>
+        <v>56</v>
       </c>
       <c r="C16" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D16" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="B17" t="s">
-        <v>45</v>
+        <v>57</v>
       </c>
       <c r="C17" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D17" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="B18" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="C18" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D18" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>51</v>
+        <v>31</v>
       </c>
       <c r="B19" t="s">
-        <v>49</v>
+        <v>32</v>
       </c>
       <c r="C19" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D19" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>54</v>
+        <v>34</v>
       </c>
       <c r="B20" t="s">
-        <v>52</v>
+        <v>33</v>
       </c>
       <c r="C20" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D20" t="s">
-        <v>58</v>
+        <v>46</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>35</v>
+      </c>
+      <c r="B21" t="s">
+        <v>36</v>
+      </c>
+      <c r="C21" t="s">
+        <v>13</v>
+      </c>
+      <c r="D21" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>40</v>
+      </c>
+      <c r="B22" t="s">
+        <v>38</v>
+      </c>
+      <c r="C22" t="s">
+        <v>13</v>
+      </c>
+      <c r="D22" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>41</v>
+      </c>
+      <c r="B23" t="s">
+        <v>39</v>
+      </c>
+      <c r="C23" t="s">
+        <v>13</v>
+      </c>
+      <c r="D23" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>44</v>
+      </c>
+      <c r="B24" t="s">
+        <v>42</v>
+      </c>
+      <c r="C24" t="s">
+        <v>13</v>
+      </c>
+      <c r="D24" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>